<commit_message>
Add result saver as xlsx
Use xlsxwriter to build xlsx file
</commit_message>
<xml_diff>
--- a/Test Result Sample.xlsx
+++ b/Test Result Sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -97,7 +97,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="yyyy/m/d\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +123,13 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -258,8 +268,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -269,40 +306,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,14 +601,14 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:J36"/>
+      <selection activeCell="A6" sqref="A6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
@@ -604,599 +617,569 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="J31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="J32:J36"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="J20:J24"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="I8:I12"/>
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="D2:E2"/>
@@ -1210,6 +1193,36 @@
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I8:I12"/>
+    <mergeCell ref="J8:J12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="J14:J18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="I32:I36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>